<commit_message>
Finished BOM + swapped front panel picture
</commit_message>
<xml_diff>
--- a/BOM/Pulseblaster_Clock_Source_BOM.xlsx
+++ b/BOM/Pulseblaster_Clock_Source_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhc83\OneDrive - The University of Chicago\Desktop\FrAg Code\pulseblaster-clock-source\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBBC195-9191-4987-99CD-29B32242757C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F8C677-8AED-4146-A308-FA4441BFF900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2610" windowWidth="21840" windowHeight="13020" xr2:uid="{BF4B63C3-1382-42E3-A180-6A07441C795C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>Part</t>
   </si>
@@ -77,42 +77,9 @@
     <t>Green banana jack</t>
   </si>
   <si>
-    <t>1195-6784-ND</t>
-  </si>
-  <si>
-    <t>1688-1219-ND</t>
-  </si>
-  <si>
-    <t>Panel mount USB to USB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For connecting to the synthHD </t>
-  </si>
-  <si>
-    <t>Regulated Power Distribution Rev A</t>
-  </si>
-  <si>
-    <t>Regulator circuit</t>
-  </si>
-  <si>
-    <t>DeMille Lab</t>
-  </si>
-  <si>
-    <t>Used lab regulated-power-distribution circuit</t>
-  </si>
-  <si>
     <t>Total cost</t>
   </si>
   <si>
-    <t>ACX1567-ND</t>
-  </si>
-  <si>
-    <t>Note: This BOM does NOT include the minicircuits SMA cables or RF adapters. Use whatever sizes work for you. I mainly used 4", 6", and 8"</t>
-  </si>
-  <si>
-    <t>For connecting RF switch TTL to the front panel</t>
-  </si>
-  <si>
     <t>296-38479-ND</t>
   </si>
   <si>
@@ -143,24 +110,12 @@
     <t>5073-LCAD30013-ND</t>
   </si>
   <si>
-    <t>Panel mount BNC to SMA</t>
-  </si>
-  <si>
-    <t>For 50 MHz</t>
-  </si>
-  <si>
     <t xml:space="preserve"> NB3N3020DTGEVB </t>
   </si>
   <si>
     <t>Clock Multiplier Evaluation Board</t>
   </si>
   <si>
-    <t>SMA cables</t>
-  </si>
-  <si>
-    <t>Caps/JST for power distribution</t>
-  </si>
-  <si>
     <t>ACX1326-ND</t>
   </si>
   <si>
@@ -198,6 +153,72 @@
   </si>
   <si>
     <t>108-0904-001</t>
+  </si>
+  <si>
+    <t>RM1U1908SBK</t>
+  </si>
+  <si>
+    <t>1 for clock out, 7 for 10 MHz LVTTL out, 1 for pulseblasters</t>
+  </si>
+  <si>
+    <t>Larger panel mount BNC to SMA</t>
+  </si>
+  <si>
+    <t>For 4x 50 MHz clock out</t>
+  </si>
+  <si>
+    <t>LCAD30013</t>
+  </si>
+  <si>
+    <t>LD1117V33C</t>
+  </si>
+  <si>
+    <t>CUSTOM</t>
+  </si>
+  <si>
+    <t>buffer_pcb</t>
+  </si>
+  <si>
+    <t>CeNTREX buffer PCB</t>
+  </si>
+  <si>
+    <t>Note: Has different pinout than standard LM78xx. I also used a 100 nF input filter cap and 10uF output filter cap as per datasheet</t>
+  </si>
+  <si>
+    <t>3272-CO-174SMAX200-000.6-ND</t>
+  </si>
+  <si>
+    <t>6" SMA cable</t>
+  </si>
+  <si>
+    <t>12" SMA cable</t>
+  </si>
+  <si>
+    <t>3272-CO-174SMAX200-001-ND</t>
+  </si>
+  <si>
+    <t>CO-174SMAx200-001</t>
+  </si>
+  <si>
+    <t>CO-174SMAx200-000.6</t>
+  </si>
+  <si>
+    <t>Other equivalent cables work</t>
+  </si>
+  <si>
+    <t>SMA male-to-male adapter</t>
+  </si>
+  <si>
+    <t>Any equivalent model works</t>
+  </si>
+  <si>
+    <t>ADP-SMAM-SMAM-ND</t>
+  </si>
+  <si>
+    <t>Breadboard</t>
+  </si>
+  <si>
+    <t>For soldering 3.3V regulator + voltage divider to generate 1.65V</t>
   </si>
 </sst>
 </file>
@@ -223,28 +244,25 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -259,28 +277,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F35643-220C-4CEB-88C9-5CBB078B24A8}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,421 +620,450 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
     <col min="5" max="6" width="14.42578125" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="7">
+    <row r="2" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6">
         <v>178.8</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>1</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="2">
+      <c r="G2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="6">
         <f>E2*F2</f>
         <v>178.8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="2">
+    <row r="3" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="6">
         <v>400</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="G3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6">
         <f>E3*F3</f>
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2">
+    <row r="4" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6">
         <v>178.8</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="6">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" ref="H3:H5" si="0">E4*F4</f>
+      <c r="G4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H5" si="0">E4*F4</f>
         <v>178.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="6">
         <v>1.53</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="6">
         <v>1.53</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6">
         <f t="shared" ref="H6" si="1">E6*F6</f>
         <v>1.53</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="F7" s="6">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
+      <c r="G7" s="6"/>
+      <c r="H7" s="6">
         <f t="shared" ref="H7:H16" si="2">E7*F7</f>
+        <v>150.19999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>242181</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="6">
+        <v>30.88</v>
+      </c>
+      <c r="F8" s="6">
+        <v>9</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="2"/>
+        <v>277.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6">
+        <v>22.66</v>
+      </c>
+      <c r="F9" s="6">
+        <v>4</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="2"/>
+        <v>90.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6">
+        <v>13.57</v>
+      </c>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="2"/>
+        <v>108.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="6">
+        <v>13.81</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="2"/>
+        <v>69.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5.31</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="2"/>
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="2"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="2">
-        <v>15.67</v>
-      </c>
-      <c r="F8" s="2">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <f t="shared" si="2"/>
-        <v>156.69999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1.19</v>
-      </c>
-      <c r="F9" s="2">
-        <v>3</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <f t="shared" si="2"/>
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2">
-        <v>1.27</v>
-      </c>
-      <c r="F10" s="2">
-        <v>4</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10" s="2">
-        <f t="shared" si="2"/>
-        <v>5.08</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2">
-        <v>16.29</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="F14" s="6">
         <v>2</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="2">
-        <f t="shared" si="2"/>
-        <v>32.58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="G14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2">
-        <v>26.05</v>
-      </c>
-      <c r="F14" s="2">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="6">
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
         <v>1</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="2">
-        <f t="shared" si="2"/>
-        <v>26.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="G15" s="4"/>
+      <c r="H15" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
+    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="2">
-        <f>SUM(H3:H16)</f>
-        <v>805.84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>40</v>
+      <c r="G18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="1">
+        <f ca="1">SUM(H3:H18)</f>
+        <v>1127.3100000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>